<commit_message>
Add file via uploading
</commit_message>
<xml_diff>
--- a/PSP_Sheets/1_3_PSP_Sheet_이상우.xlsx
+++ b/PSP_Sheets/1_3_PSP_Sheet_이상우.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOGANG\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="작성자명" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1496,6 +1496,214 @@
         <charset val="129"/>
       </rPr>
       <t>제작</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설문지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>자료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정리</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>설문지 자료 토대로 Initial Data set 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 29</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>web1 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>web1 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1503,7 +1711,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
@@ -2082,7 +2290,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2461,36 +2669,84 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="4"/>
+      <c r="A22" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D22" s="9">
+        <v>20</v>
+      </c>
+      <c r="E22" s="16">
+        <v>150</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="18"/>
+      <c r="A23" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="D23" s="9">
+        <v>70</v>
+      </c>
+      <c r="E23" s="16">
+        <v>469</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="4"/>
+      <c r="A24" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16">
+        <v>120</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="4"/>
+      <c r="A25" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.16388888888888889</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="16">
+        <v>236</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21"/>

</xml_diff>